<commit_message>
admin and user page is complete
</commit_message>
<xml_diff>
--- a/uploads/icon.xlsx
+++ b/uploads/icon.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="373">
   <si>
     <t>OWNER NAME</t>
   </si>
@@ -1117,12 +1117,34 @@
   </si>
   <si>
     <t>DLF Icon</t>
+  </si>
+  <si>
+    <t>REMARK</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>cedwe</t>
+  </si>
+  <si>
+    <t>hded</t>
+  </si>
+  <si>
+    <t>ucdehowj[</t>
+  </si>
+  <si>
+    <t>uidheoiwfuihwiudhuifhwdeuifhewfiuehfuidhweu</t>
+  </si>
+  <si>
+    <t>dehfwbuidfheoiwuhdoi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -1532,7 +1554,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1540,7 +1562,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B383"/>
+  <dimension ref="A1:C383"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
@@ -1548,8 +1570,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="50.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="12" style="7" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="50.5703125"/>
+    <col min="2" max="2" customWidth="true" style="7" width="12.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21" customHeight="1">
@@ -1565,6 +1587,9 @@
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="C2" t="s" s="0">
+        <v>366</v>
+      </c>
     </row>
     <row r="3" spans="1:2" ht="21" customHeight="1">
       <c r="A3" s="3" t="s">
@@ -1573,6 +1598,9 @@
       <c r="B3" s="6">
         <v>8527540740</v>
       </c>
+      <c r="C3" t="s" s="0">
+        <v>367</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="21" customHeight="1">
       <c r="A4" s="3" t="s">
@@ -1586,6 +1614,9 @@
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="C5" t="s" s="0">
+        <v>368</v>
+      </c>
     </row>
     <row r="6" spans="1:2" ht="21" customHeight="1">
       <c r="A6" s="3" t="s">
@@ -1594,6 +1625,9 @@
       <c r="B6" s="6">
         <v>8874202160</v>
       </c>
+      <c r="C6" t="s" s="0">
+        <v>369</v>
+      </c>
     </row>
     <row r="7" spans="1:2" ht="21" customHeight="1">
       <c r="A7" s="3" t="s">
@@ -1602,6 +1636,9 @@
       <c r="B7" s="6">
         <v>9810391361</v>
       </c>
+      <c r="C7" t="s" s="0">
+        <v>370</v>
+      </c>
     </row>
     <row r="8" spans="1:2" ht="21" customHeight="1">
       <c r="A8" s="3" t="s">
@@ -1610,6 +1647,9 @@
       <c r="B8" s="6">
         <v>9810082711</v>
       </c>
+      <c r="C8" t="s" s="0">
+        <v>371</v>
+      </c>
     </row>
     <row r="9" spans="1:2" ht="21" customHeight="1">
       <c r="A9" s="3" t="s">
@@ -1617,6 +1657,9 @@
       </c>
       <c r="B9" s="6">
         <v>9810000721</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>372</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="21" customHeight="1">

</xml_diff>

<commit_message>
now this time is update code for mobile app and web app
</commit_message>
<xml_diff>
--- a/uploads/icon.xlsx
+++ b/uploads/icon.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="370">
   <si>
     <t>OWNER NAME</t>
   </si>
@@ -1119,25 +1119,17 @@
     <t>DLF Icon</t>
   </si>
   <si>
-    <t>REMARK</t>
-  </si>
-  <si>
-    <t>hello</t>
-  </si>
-  <si>
-    <t>cedwe</t>
-  </si>
-  <si>
-    <t>hded</t>
-  </si>
-  <si>
-    <t>ucdehowj[</t>
-  </si>
-  <si>
-    <t>uidheoiwfuihwiudhuifhwdeuifhewfiuehfuidhweu</t>
-  </si>
-  <si>
-    <t>dehfwbuidfheoiwuhdoi</t>
+    <t>hhoyhjs</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t xml:space="preserve">Remarks
+</t>
+  </si>
+  <si>
+    <t>Remarks</t>
   </si>
 </sst>
 </file>
@@ -1579,6 +1571,9 @@
         <v>365</v>
       </c>
       <c r="B1" s="10"/>
+      <c r="C1" t="s" s="0">
+        <v>368</v>
+      </c>
     </row>
     <row r="2" spans="1:2" s="1" customFormat="1" ht="21" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -1588,7 +1583,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="21" customHeight="1">
@@ -1599,7 +1594,7 @@
         <v>8527540740</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="21" customHeight="1">
@@ -1609,14 +1604,14 @@
       <c r="B4" s="6">
         <v>9811391047</v>
       </c>
+      <c r="C4" t="s" s="0">
+        <v>367</v>
+      </c>
     </row>
     <row r="5" spans="1:2" ht="21" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s" s="0">
-        <v>368</v>
-      </c>
     </row>
     <row r="6" spans="1:2" ht="21" customHeight="1">
       <c r="A6" s="3" t="s">
@@ -1626,7 +1621,7 @@
         <v>8874202160</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="21" customHeight="1">
@@ -1636,9 +1631,6 @@
       <c r="B7" s="6">
         <v>9810391361</v>
       </c>
-      <c r="C7" t="s" s="0">
-        <v>370</v>
-      </c>
     </row>
     <row r="8" spans="1:2" ht="21" customHeight="1">
       <c r="A8" s="3" t="s">
@@ -1647,9 +1639,6 @@
       <c r="B8" s="6">
         <v>9810082711</v>
       </c>
-      <c r="C8" t="s" s="0">
-        <v>371</v>
-      </c>
     </row>
     <row r="9" spans="1:2" ht="21" customHeight="1">
       <c r="A9" s="3" t="s">
@@ -1657,9 +1646,6 @@
       </c>
       <c r="B9" s="6">
         <v>9810000721</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>372</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="21" customHeight="1">

</xml_diff>